<commit_message>
👽 Updated code font
</commit_message>
<xml_diff>
--- a/assets/tools/_unit-calculations.xlsx
+++ b/assets/tools/_unit-calculations.xlsx
@@ -1,18 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="940" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="940" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="px as pt" sheetId="1" r:id="rId1"/>
     <sheet name="Fractions as %" sheetId="2" r:id="rId2"/>
     <sheet name="scss Fx" sheetId="5" r:id="rId3"/>
     <sheet name="@media (working)" sheetId="4" r:id="rId4"/>
-    <sheet name="Gray Values" sheetId="6" r:id="rId5"/>
-    <sheet name="@media zzOLD" sheetId="7" r:id="rId6"/>
+    <sheet name="Base Colours" sheetId="8" r:id="rId5"/>
+    <sheet name="Gray Values" sheetId="6" r:id="rId6"/>
+    <sheet name="@media zzOLD" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="190">
   <si>
     <t>css-pixels-per-point</t>
   </si>
@@ -366,6 +367,234 @@
   </si>
   <si>
     <t>baseline in points</t>
+  </si>
+  <si>
+    <t>Base colour source: http://www.color-hex.com/color/ffd700</t>
+  </si>
+  <si>
+    <t>-add1</t>
+  </si>
+  <si>
+    <t>-add2</t>
+  </si>
+  <si>
+    <t>-add3</t>
+  </si>
+  <si>
+    <t>-add4</t>
+  </si>
+  <si>
+    <t>-add5</t>
+  </si>
+  <si>
+    <t>-add6</t>
+  </si>
+  <si>
+    <t>-add7</t>
+  </si>
+  <si>
+    <t>-add8</t>
+  </si>
+  <si>
+    <t>-add9</t>
+  </si>
+  <si>
+    <t>-add10</t>
+  </si>
+  <si>
+    <t>-sub10</t>
+  </si>
+  <si>
+    <t>-sub9</t>
+  </si>
+  <si>
+    <t>-sub8</t>
+  </si>
+  <si>
+    <t>-sub1</t>
+  </si>
+  <si>
+    <t>-sub2</t>
+  </si>
+  <si>
+    <t>-sub3</t>
+  </si>
+  <si>
+    <t>-sub4</t>
+  </si>
+  <si>
+    <t>-sub5</t>
+  </si>
+  <si>
+    <t>-sub6</t>
+  </si>
+  <si>
+    <t>-sub7</t>
+  </si>
+  <si>
+    <t>#ffd700</t>
+  </si>
+  <si>
+    <t>#e5c100</t>
+  </si>
+  <si>
+    <t>#ccac00</t>
+  </si>
+  <si>
+    <t>#b29600</t>
+  </si>
+  <si>
+    <t>#998100</t>
+  </si>
+  <si>
+    <t>#7f6b00</t>
+  </si>
+  <si>
+    <t>#665600</t>
+  </si>
+  <si>
+    <t>#4c4000</t>
+  </si>
+  <si>
+    <t>#332b00</t>
+  </si>
+  <si>
+    <t>#191500</t>
+  </si>
+  <si>
+    <t>#000000</t>
+  </si>
+  <si>
+    <t>#ffdb19</t>
+  </si>
+  <si>
+    <t>#ffdf32</t>
+  </si>
+  <si>
+    <t>#ffe34c</t>
+  </si>
+  <si>
+    <t>#ffe766</t>
+  </si>
+  <si>
+    <t>#ffeb7f</t>
+  </si>
+  <si>
+    <t>#ffef99</t>
+  </si>
+  <si>
+    <t>#fff3b2</t>
+  </si>
+  <si>
+    <t>#fff7cc</t>
+  </si>
+  <si>
+    <t>#fffbe5</t>
+  </si>
+  <si>
+    <t>#ffffff</t>
+  </si>
+  <si>
+    <t>BASE</t>
+  </si>
+  <si>
+    <t>BUFF</t>
+  </si>
+  <si>
+    <t>#fff8e4</t>
+  </si>
+  <si>
+    <t>#fff8e6</t>
+  </si>
+  <si>
+    <t>#fff9e9</t>
+  </si>
+  <si>
+    <t>#fffaec</t>
+  </si>
+  <si>
+    <t>#fffaee</t>
+  </si>
+  <si>
+    <t>#fffbf1</t>
+  </si>
+  <si>
+    <t>#fffcf4</t>
+  </si>
+  <si>
+    <t>#fffcf6</t>
+  </si>
+  <si>
+    <t>#fffdf9</t>
+  </si>
+  <si>
+    <t>#fffefc</t>
+  </si>
+  <si>
+    <t>#e5dfcd</t>
+  </si>
+  <si>
+    <t>Base colour source: http://www.color-hex.com/color/fff8e4</t>
+  </si>
+  <si>
+    <t>#fbddaa</t>
+  </si>
+  <si>
+    <t>#fbe0b2</t>
+  </si>
+  <si>
+    <t>#fbe3bb</t>
+  </si>
+  <si>
+    <t>#fce7c3</t>
+  </si>
+  <si>
+    <t>#fceacc</t>
+  </si>
+  <si>
+    <t>#fdeed4</t>
+  </si>
+  <si>
+    <t>#fdf1dd</t>
+  </si>
+  <si>
+    <t>#fdf4e5</t>
+  </si>
+  <si>
+    <t>#fef8ee</t>
+  </si>
+  <si>
+    <t>#fefbf6</t>
+  </si>
+  <si>
+    <t>#e1c699</t>
+  </si>
+  <si>
+    <t>#c8b088</t>
+  </si>
+  <si>
+    <t>#af9a76</t>
+  </si>
+  <si>
+    <t>#968466</t>
+  </si>
+  <si>
+    <t>#7d6e55</t>
+  </si>
+  <si>
+    <t>#645844</t>
+  </si>
+  <si>
+    <t>#4b4233</t>
+  </si>
+  <si>
+    <t>#322c22</t>
+  </si>
+  <si>
+    <t>#191611</t>
+  </si>
+  <si>
+    <t>Base colour source: http://www.color-hex.com/color/fbddaa</t>
   </si>
 </sst>
 </file>
@@ -377,7 +606,7 @@
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -438,6 +667,39 @@
     </font>
     <font>
       <sz val="9"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+    </font>
+    <font>
+      <sz val="13.35"/>
+      <color theme="1"/>
+      <name val="Avenir Book"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="13.35"/>
+      <color theme="10"/>
+      <name val="Avenir Book"/>
+    </font>
+    <font>
+      <sz val="13.35"/>
+      <color rgb="FF000000"/>
+      <name val="Avenir Book"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13.35"/>
       <color theme="1"/>
       <name val="Avenir Book"/>
     </font>
@@ -716,7 +978,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="77">
+  <cellStyleXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -794,8 +1056,51 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1154,6 +1459,27 @@
     <xf numFmtId="13" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1190,29 +1516,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="77">
+  <cellStyles count="120">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1288,6 +1618,49 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -6052,12 +6425,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:W446"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6580" ySplit="3480" topLeftCell="J18" activePane="bottomRight"/>
-      <selection activeCell="I9" sqref="I9"/>
-      <selection pane="topRight" activeCell="M1" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
-      <selection pane="bottomRight" activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3480" topLeftCell="A18" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0"/>
@@ -6123,14 +6493,14 @@
       </c>
     </row>
     <row r="7" spans="3:23" ht="40" customHeight="1">
-      <c r="D7" s="122" t="s">
+      <c r="D7" s="129" t="s">
         <v>110</v>
       </c>
-      <c r="E7" s="122" t="s">
+      <c r="E7" s="129" t="s">
         <v>111</v>
       </c>
       <c r="F7" s="60"/>
-      <c r="G7" s="136">
+      <c r="G7" s="124">
         <v>7</v>
       </c>
       <c r="H7" s="113">
@@ -6182,10 +6552,10 @@
     </row>
     <row r="8" spans="3:23" ht="40" customHeight="1">
       <c r="C8" s="121"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="130"/>
       <c r="F8" s="61"/>
-      <c r="G8" s="137">
+      <c r="G8" s="125">
         <f>G7+(6.3/16)</f>
         <v>7.3937499999999998</v>
       </c>
@@ -6238,10 +6608,10 @@
       </c>
     </row>
     <row r="9" spans="3:23" ht="40" customHeight="1">
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
+      <c r="D9" s="130"/>
+      <c r="E9" s="130"/>
       <c r="F9" s="61"/>
-      <c r="G9" s="137">
+      <c r="G9" s="125">
         <f>G8+(6.3/16)</f>
         <v>7.7874999999999996</v>
       </c>
@@ -6283,10 +6653,10 @@
       <c r="W9" s="43"/>
     </row>
     <row r="10" spans="3:23" ht="40" customHeight="1">
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
       <c r="F10" s="61"/>
-      <c r="G10" s="137">
+      <c r="G10" s="125">
         <f t="shared" ref="G10:G32" si="6">G9+(6.3/16)</f>
         <v>8.1812500000000004</v>
       </c>
@@ -6339,10 +6709,10 @@
       </c>
     </row>
     <row r="11" spans="3:23" ht="40" customHeight="1" thickBot="1">
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="130"/>
       <c r="F11" s="61"/>
-      <c r="G11" s="137">
+      <c r="G11" s="125">
         <f t="shared" si="6"/>
         <v>8.5750000000000011</v>
       </c>
@@ -6395,10 +6765,10 @@
       </c>
     </row>
     <row r="12" spans="3:23" ht="40" customHeight="1">
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
+      <c r="D12" s="130"/>
+      <c r="E12" s="130"/>
       <c r="F12" s="61"/>
-      <c r="G12" s="137">
+      <c r="G12" s="125">
         <f t="shared" si="6"/>
         <v>8.9687500000000018</v>
       </c>
@@ -6436,10 +6806,10 @@
       <c r="R12" s="59"/>
     </row>
     <row r="13" spans="3:23" ht="40" customHeight="1">
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
+      <c r="D13" s="130"/>
+      <c r="E13" s="130"/>
       <c r="F13" s="61"/>
-      <c r="G13" s="137">
+      <c r="G13" s="125">
         <f t="shared" si="6"/>
         <v>9.3625000000000025</v>
       </c>
@@ -6477,10 +6847,10 @@
       <c r="R13" s="59"/>
     </row>
     <row r="14" spans="3:23" ht="40" customHeight="1">
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
+      <c r="D14" s="130"/>
+      <c r="E14" s="130"/>
       <c r="F14" s="61"/>
-      <c r="G14" s="137">
+      <c r="G14" s="125">
         <f t="shared" si="6"/>
         <v>9.7562500000000032</v>
       </c>
@@ -6518,10 +6888,10 @@
       <c r="R14" s="59"/>
     </row>
     <row r="15" spans="3:23" ht="40" customHeight="1">
-      <c r="D15" s="123"/>
-      <c r="E15" s="123"/>
+      <c r="D15" s="130"/>
+      <c r="E15" s="130"/>
       <c r="F15" s="61"/>
-      <c r="G15" s="137">
+      <c r="G15" s="125">
         <f t="shared" si="6"/>
         <v>10.150000000000004</v>
       </c>
@@ -6559,10 +6929,10 @@
       <c r="R15" s="59"/>
     </row>
     <row r="16" spans="3:23" ht="40" customHeight="1">
-      <c r="D16" s="123"/>
-      <c r="E16" s="123"/>
+      <c r="D16" s="130"/>
+      <c r="E16" s="130"/>
       <c r="F16" s="61"/>
-      <c r="G16" s="137">
+      <c r="G16" s="125">
         <f t="shared" si="6"/>
         <v>10.543750000000005</v>
       </c>
@@ -6600,10 +6970,10 @@
       <c r="R16" s="59"/>
     </row>
     <row r="17" spans="4:21" ht="40" customHeight="1">
-      <c r="D17" s="123"/>
-      <c r="E17" s="123"/>
+      <c r="D17" s="130"/>
+      <c r="E17" s="130"/>
       <c r="F17" s="61"/>
-      <c r="G17" s="137">
+      <c r="G17" s="125">
         <f t="shared" si="6"/>
         <v>10.937500000000005</v>
       </c>
@@ -6641,10 +7011,10 @@
       <c r="R17" s="59"/>
     </row>
     <row r="18" spans="4:21" ht="40" customHeight="1">
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="130"/>
       <c r="F18" s="61"/>
-      <c r="G18" s="137">
+      <c r="G18" s="125">
         <f t="shared" si="6"/>
         <v>11.331250000000006</v>
       </c>
@@ -6682,10 +7052,10 @@
       <c r="R18" s="59"/>
     </row>
     <row r="19" spans="4:21" ht="40" customHeight="1">
-      <c r="D19" s="123"/>
-      <c r="E19" s="123"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130"/>
       <c r="F19" s="61"/>
-      <c r="G19" s="137">
+      <c r="G19" s="125">
         <f t="shared" si="6"/>
         <v>11.725000000000007</v>
       </c>
@@ -6726,10 +7096,10 @@
       <c r="U19" s="22"/>
     </row>
     <row r="20" spans="4:21" ht="40" customHeight="1">
-      <c r="D20" s="123"/>
-      <c r="E20" s="123"/>
+      <c r="D20" s="130"/>
+      <c r="E20" s="130"/>
       <c r="F20" s="61"/>
-      <c r="G20" s="137">
+      <c r="G20" s="125">
         <f t="shared" si="6"/>
         <v>12.118750000000007</v>
       </c>
@@ -6770,10 +7140,10 @@
       <c r="U20" s="22"/>
     </row>
     <row r="21" spans="4:21" ht="40" customHeight="1">
-      <c r="D21" s="123"/>
-      <c r="E21" s="123"/>
+      <c r="D21" s="130"/>
+      <c r="E21" s="130"/>
       <c r="F21" s="61"/>
-      <c r="G21" s="138">
+      <c r="G21" s="126">
         <f t="shared" si="6"/>
         <v>12.512500000000008</v>
       </c>
@@ -6813,10 +7183,10 @@
       <c r="U21" s="22"/>
     </row>
     <row r="22" spans="4:21" ht="42" customHeight="1">
-      <c r="D22" s="123"/>
-      <c r="E22" s="123"/>
+      <c r="D22" s="130"/>
+      <c r="E22" s="130"/>
       <c r="F22" s="100"/>
-      <c r="G22" s="137">
+      <c r="G22" s="125">
         <f t="shared" si="6"/>
         <v>12.906250000000009</v>
       </c>
@@ -6857,10 +7227,10 @@
       <c r="U22" s="22"/>
     </row>
     <row r="23" spans="4:21" ht="40" customHeight="1">
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
+      <c r="D23" s="130"/>
+      <c r="E23" s="130"/>
       <c r="F23" s="101"/>
-      <c r="G23" s="139">
+      <c r="G23" s="127">
         <f t="shared" si="6"/>
         <v>13.30000000000001</v>
       </c>
@@ -6888,7 +7258,7 @@
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="N23" s="135">
+      <c r="N23" s="123">
         <f t="shared" si="5"/>
         <v>17.300000000000011</v>
       </c>
@@ -6901,10 +7271,10 @@
       <c r="U23" s="22"/>
     </row>
     <row r="24" spans="4:21" ht="40" customHeight="1">
-      <c r="D24" s="123"/>
-      <c r="E24" s="123"/>
+      <c r="D24" s="130"/>
+      <c r="E24" s="130"/>
       <c r="F24" s="101"/>
-      <c r="G24" s="137">
+      <c r="G24" s="125">
         <f t="shared" si="6"/>
         <v>13.69375000000001</v>
       </c>
@@ -6945,10 +7315,10 @@
       <c r="U24" s="22"/>
     </row>
     <row r="25" spans="4:21" ht="40" customHeight="1">
-      <c r="D25" s="123"/>
-      <c r="E25" s="123"/>
+      <c r="D25" s="130"/>
+      <c r="E25" s="130"/>
       <c r="F25" s="101"/>
-      <c r="G25" s="138">
+      <c r="G25" s="126">
         <f t="shared" si="6"/>
         <v>14.087500000000011</v>
       </c>
@@ -6989,10 +7359,10 @@
       <c r="U25" s="22"/>
     </row>
     <row r="26" spans="4:21" ht="40" customHeight="1">
-      <c r="D26" s="123"/>
-      <c r="E26" s="123"/>
+      <c r="D26" s="130"/>
+      <c r="E26" s="130"/>
       <c r="F26" s="101"/>
-      <c r="G26" s="137">
+      <c r="G26" s="125">
         <f t="shared" si="6"/>
         <v>14.481250000000012</v>
       </c>
@@ -7033,10 +7403,10 @@
       <c r="U26" s="22"/>
     </row>
     <row r="27" spans="4:21" ht="40" customHeight="1">
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
+      <c r="D27" s="130"/>
+      <c r="E27" s="130"/>
       <c r="F27" s="101"/>
-      <c r="G27" s="138">
+      <c r="G27" s="126">
         <f t="shared" si="6"/>
         <v>14.875000000000012</v>
       </c>
@@ -7077,10 +7447,10 @@
       <c r="U27" s="22"/>
     </row>
     <row r="28" spans="4:21" ht="40" customHeight="1">
-      <c r="D28" s="123"/>
-      <c r="E28" s="123"/>
+      <c r="D28" s="130"/>
+      <c r="E28" s="130"/>
       <c r="F28" s="101"/>
-      <c r="G28" s="137">
+      <c r="G28" s="125">
         <f t="shared" si="6"/>
         <v>15.268750000000013</v>
       </c>
@@ -7118,10 +7488,10 @@
       <c r="R28" s="59"/>
     </row>
     <row r="29" spans="4:21" ht="40" customHeight="1">
-      <c r="D29" s="123"/>
-      <c r="E29" s="123"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="130"/>
       <c r="F29" s="101"/>
-      <c r="G29" s="138">
+      <c r="G29" s="126">
         <f t="shared" si="6"/>
         <v>15.662500000000014</v>
       </c>
@@ -7159,10 +7529,10 @@
       <c r="R29" s="59"/>
     </row>
     <row r="30" spans="4:21" ht="40" customHeight="1">
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
+      <c r="D30" s="130"/>
+      <c r="E30" s="130"/>
       <c r="F30" s="101"/>
-      <c r="G30" s="138">
+      <c r="G30" s="126">
         <f t="shared" si="6"/>
         <v>16.056250000000013</v>
       </c>
@@ -7200,10 +7570,10 @@
       <c r="R30" s="59"/>
     </row>
     <row r="31" spans="4:21" ht="40" customHeight="1">
-      <c r="D31" s="123"/>
-      <c r="E31" s="123"/>
+      <c r="D31" s="130"/>
+      <c r="E31" s="130"/>
       <c r="F31" s="101"/>
-      <c r="G31" s="137">
+      <c r="G31" s="125">
         <f t="shared" si="6"/>
         <v>16.450000000000014</v>
       </c>
@@ -7241,10 +7611,10 @@
       <c r="R31" s="59"/>
     </row>
     <row r="32" spans="4:21" ht="40" customHeight="1" thickBot="1">
-      <c r="D32" s="123"/>
-      <c r="E32" s="123"/>
+      <c r="D32" s="130"/>
+      <c r="E32" s="130"/>
       <c r="F32" s="101"/>
-      <c r="G32" s="140">
+      <c r="G32" s="128">
         <f t="shared" si="6"/>
         <v>16.843750000000014</v>
       </c>
@@ -7272,7 +7642,7 @@
         <f t="shared" si="7"/>
         <v>6.25</v>
       </c>
-      <c r="N32" s="134">
+      <c r="N32" s="122">
         <f t="shared" si="5"/>
         <v>23.093750000000014</v>
       </c>
@@ -10429,6 +10799,484 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K18" activeCellId="2" sqref="E18 H18 K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="16384" width="10.625" style="141"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:14" ht="19">
+      <c r="A2" s="146"/>
+      <c r="B2" s="147" t="s">
+        <v>114</v>
+      </c>
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="146"/>
+      <c r="F2" s="146"/>
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+    </row>
+    <row r="3" spans="1:14" ht="19">
+      <c r="A3" s="146"/>
+      <c r="B3" s="146"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="146"/>
+      <c r="E3" s="146"/>
+      <c r="F3" s="146"/>
+      <c r="G3" s="146"/>
+      <c r="H3" s="146"/>
+      <c r="I3" s="146"/>
+      <c r="J3" s="146"/>
+      <c r="K3" s="146"/>
+      <c r="L3" s="146"/>
+    </row>
+    <row r="4" spans="1:14" s="142" customFormat="1" ht="38" customHeight="1">
+      <c r="A4" s="148"/>
+      <c r="B4" s="148">
+        <v>0</v>
+      </c>
+      <c r="C4" s="149" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="150" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="149" t="s">
+        <v>130</v>
+      </c>
+      <c r="F4" s="149" t="s">
+        <v>131</v>
+      </c>
+      <c r="G4" s="150" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="149" t="s">
+        <v>133</v>
+      </c>
+      <c r="I4" s="149" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="150" t="s">
+        <v>127</v>
+      </c>
+      <c r="K4" s="149" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="149" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="142" customFormat="1" ht="38" customHeight="1">
+      <c r="A5" s="148" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="151" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="148" t="s">
+        <v>136</v>
+      </c>
+      <c r="D5" s="148" t="s">
+        <v>137</v>
+      </c>
+      <c r="E5" s="151" t="s">
+        <v>138</v>
+      </c>
+      <c r="F5" s="148" t="s">
+        <v>139</v>
+      </c>
+      <c r="G5" s="148" t="s">
+        <v>140</v>
+      </c>
+      <c r="H5" s="151" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" s="148" t="s">
+        <v>142</v>
+      </c>
+      <c r="J5" s="148" t="s">
+        <v>143</v>
+      </c>
+      <c r="K5" s="151" t="s">
+        <v>144</v>
+      </c>
+      <c r="L5" s="148" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="142" customFormat="1" ht="38" customHeight="1">
+      <c r="A6" s="148" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" s="151" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="148" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6" s="148" t="s">
+        <v>147</v>
+      </c>
+      <c r="E6" s="151" t="s">
+        <v>148</v>
+      </c>
+      <c r="F6" s="148" t="s">
+        <v>149</v>
+      </c>
+      <c r="G6" s="148" t="s">
+        <v>150</v>
+      </c>
+      <c r="H6" s="151" t="s">
+        <v>151</v>
+      </c>
+      <c r="I6" s="148" t="s">
+        <v>152</v>
+      </c>
+      <c r="J6" s="148" t="s">
+        <v>153</v>
+      </c>
+      <c r="K6" s="151" t="s">
+        <v>154</v>
+      </c>
+      <c r="L6" s="148" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="142" customFormat="1" ht="38" customHeight="1">
+      <c r="A7" s="148"/>
+      <c r="B7" s="148">
+        <v>0</v>
+      </c>
+      <c r="C7" s="149" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="149" t="s">
+        <v>116</v>
+      </c>
+      <c r="E7" s="149" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" s="149" t="s">
+        <v>118</v>
+      </c>
+      <c r="G7" s="149" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="149" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="149" t="s">
+        <v>121</v>
+      </c>
+      <c r="J7" s="149" t="s">
+        <v>122</v>
+      </c>
+      <c r="K7" s="149" t="s">
+        <v>123</v>
+      </c>
+      <c r="L7" s="149" t="s">
+        <v>124</v>
+      </c>
+      <c r="M7" s="143"/>
+      <c r="N7" s="143"/>
+    </row>
+    <row r="8" spans="1:14" s="142" customFormat="1" ht="38" customHeight="1"/>
+    <row r="9" spans="1:14" s="142" customFormat="1" ht="38" customHeight="1">
+      <c r="B9" s="145" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="142" customFormat="1" ht="39" customHeight="1">
+      <c r="B10" s="142">
+        <v>0</v>
+      </c>
+      <c r="C10" s="143" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+    </row>
+    <row r="11" spans="1:14" s="142" customFormat="1" ht="39" customHeight="1">
+      <c r="A11" s="142" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="144" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="144" t="s">
+        <v>168</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+    </row>
+    <row r="12" spans="1:14" s="142" customFormat="1" ht="39" customHeight="1">
+      <c r="A12" s="142" t="s">
+        <v>157</v>
+      </c>
+      <c r="B12" s="144" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="142" t="s">
+        <v>159</v>
+      </c>
+      <c r="D12" s="142" t="s">
+        <v>160</v>
+      </c>
+      <c r="E12" s="144" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" s="142" t="s">
+        <v>162</v>
+      </c>
+      <c r="G12" s="142" t="s">
+        <v>163</v>
+      </c>
+      <c r="H12" s="144" t="s">
+        <v>164</v>
+      </c>
+      <c r="I12" s="142" t="s">
+        <v>165</v>
+      </c>
+      <c r="J12" s="142" t="s">
+        <v>166</v>
+      </c>
+      <c r="K12" s="144" t="s">
+        <v>167</v>
+      </c>
+      <c r="L12" s="142" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="142" customFormat="1" ht="39" customHeight="1">
+      <c r="B13" s="142">
+        <v>0</v>
+      </c>
+      <c r="C13" s="143" t="s">
+        <v>115</v>
+      </c>
+      <c r="D13" s="143" t="s">
+        <v>116</v>
+      </c>
+      <c r="E13" s="143" t="s">
+        <v>117</v>
+      </c>
+      <c r="F13" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="G13" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="H13" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="I13" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="J13" s="143" t="s">
+        <v>122</v>
+      </c>
+      <c r="K13" s="143" t="s">
+        <v>123</v>
+      </c>
+      <c r="L13" s="143" t="s">
+        <v>124</v>
+      </c>
+      <c r="M13" s="143"/>
+      <c r="N13" s="143"/>
+    </row>
+    <row r="14" spans="1:14" s="142" customFormat="1" ht="39" customHeight="1">
+      <c r="C14" s="143"/>
+      <c r="D14" s="143"/>
+      <c r="E14" s="143"/>
+      <c r="F14" s="143"/>
+      <c r="G14" s="143"/>
+      <c r="H14" s="143"/>
+      <c r="I14" s="143"/>
+      <c r="J14" s="143"/>
+      <c r="K14" s="143"/>
+      <c r="L14" s="143"/>
+      <c r="M14" s="143"/>
+      <c r="N14" s="143"/>
+    </row>
+    <row r="15" spans="1:14" ht="39" customHeight="1">
+      <c r="B15" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="39" customHeight="1">
+      <c r="A16" s="142"/>
+      <c r="B16" s="142">
+        <v>0</v>
+      </c>
+      <c r="C16" s="143" t="s">
+        <v>128</v>
+      </c>
+      <c r="D16" s="142"/>
+      <c r="E16" s="142"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="142"/>
+      <c r="H16" s="142"/>
+      <c r="I16" s="142"/>
+      <c r="J16" s="142"/>
+      <c r="K16" s="142"/>
+      <c r="L16" s="142"/>
+    </row>
+    <row r="17" spans="1:12" ht="39" customHeight="1">
+      <c r="A17" s="142" t="s">
+        <v>157</v>
+      </c>
+      <c r="B17" s="144" t="s">
+        <v>170</v>
+      </c>
+      <c r="C17" s="142" t="s">
+        <v>180</v>
+      </c>
+      <c r="D17" s="142" t="s">
+        <v>181</v>
+      </c>
+      <c r="E17" s="144" t="s">
+        <v>182</v>
+      </c>
+      <c r="F17" s="142" t="s">
+        <v>183</v>
+      </c>
+      <c r="G17" s="142" t="s">
+        <v>184</v>
+      </c>
+      <c r="H17" s="144" t="s">
+        <v>185</v>
+      </c>
+      <c r="I17" s="142" t="s">
+        <v>186</v>
+      </c>
+      <c r="J17" s="142" t="s">
+        <v>187</v>
+      </c>
+      <c r="K17" s="144" t="s">
+        <v>188</v>
+      </c>
+      <c r="L17" s="142" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="39" customHeight="1">
+      <c r="A18" s="142" t="s">
+        <v>157</v>
+      </c>
+      <c r="B18" s="144" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="142" t="s">
+        <v>171</v>
+      </c>
+      <c r="D18" s="142" t="s">
+        <v>172</v>
+      </c>
+      <c r="E18" s="144" t="s">
+        <v>173</v>
+      </c>
+      <c r="F18" s="142" t="s">
+        <v>174</v>
+      </c>
+      <c r="G18" s="142" t="s">
+        <v>175</v>
+      </c>
+      <c r="H18" s="144" t="s">
+        <v>176</v>
+      </c>
+      <c r="I18" s="142" t="s">
+        <v>177</v>
+      </c>
+      <c r="J18" s="142" t="s">
+        <v>178</v>
+      </c>
+      <c r="K18" s="144" t="s">
+        <v>179</v>
+      </c>
+      <c r="L18" s="142" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="39" customHeight="1">
+      <c r="A19" s="142"/>
+      <c r="B19" s="142">
+        <v>0</v>
+      </c>
+      <c r="C19" s="143" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="143" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="143" t="s">
+        <v>117</v>
+      </c>
+      <c r="F19" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="G19" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="H19" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="I19" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="J19" s="143" t="s">
+        <v>122</v>
+      </c>
+      <c r="K19" s="143" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" s="143" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="39" customHeight="1"/>
+    <row r="21" spans="1:12" ht="39" customHeight="1"/>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B9" r:id="rId2"/>
+    <hyperlink ref="B15" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:D35"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
@@ -10445,10 +11293,10 @@
   <sheetData>
     <row r="6" spans="1:4" ht="20" thickBot="1">
       <c r="B6" s="99"/>
-      <c r="C6" s="124" t="s">
+      <c r="C6" s="131" t="s">
         <v>69</v>
       </c>
-      <c r="D6" s="125"/>
+      <c r="D6" s="132"/>
     </row>
     <row r="7" spans="1:4">
       <c r="C7" s="93" t="s">
@@ -10741,7 +11589,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:V468"/>
   <sheetViews>
@@ -10812,10 +11660,10 @@
       </c>
     </row>
     <row r="7" spans="4:22" ht="40" customHeight="1">
-      <c r="D7" s="126" t="s">
+      <c r="D7" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="133" t="s">
         <v>51</v>
       </c>
       <c r="F7" s="69">
@@ -10866,8 +11714,8 @@
       </c>
     </row>
     <row r="8" spans="4:22" ht="40" customHeight="1">
-      <c r="D8" s="127"/>
-      <c r="E8" s="127"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
       <c r="F8" s="74">
         <v>7.5</v>
       </c>
@@ -10916,8 +11764,8 @@
       </c>
     </row>
     <row r="9" spans="4:22" ht="40" customHeight="1">
-      <c r="D9" s="127"/>
-      <c r="E9" s="127"/>
+      <c r="D9" s="134"/>
+      <c r="E9" s="134"/>
       <c r="F9" s="74">
         <v>8</v>
       </c>
@@ -10955,8 +11803,8 @@
       <c r="V9" s="43"/>
     </row>
     <row r="10" spans="4:22" ht="40" customHeight="1">
-      <c r="D10" s="127"/>
-      <c r="E10" s="127"/>
+      <c r="D10" s="134"/>
+      <c r="E10" s="134"/>
       <c r="F10" s="74">
         <v>8.5</v>
       </c>
@@ -11005,8 +11853,8 @@
       </c>
     </row>
     <row r="11" spans="4:22" ht="40" customHeight="1" thickBot="1">
-      <c r="D11" s="127"/>
-      <c r="E11" s="127"/>
+      <c r="D11" s="134"/>
+      <c r="E11" s="134"/>
       <c r="F11" s="74">
         <v>9</v>
       </c>
@@ -11055,8 +11903,8 @@
       </c>
     </row>
     <row r="12" spans="4:22" ht="40" customHeight="1">
-      <c r="D12" s="127"/>
-      <c r="E12" s="127"/>
+      <c r="D12" s="134"/>
+      <c r="E12" s="134"/>
       <c r="F12" s="74">
         <v>9.5</v>
       </c>
@@ -11090,8 +11938,8 @@
       <c r="Q12" s="59"/>
     </row>
     <row r="13" spans="4:22" ht="40" customHeight="1">
-      <c r="D13" s="127"/>
-      <c r="E13" s="127"/>
+      <c r="D13" s="134"/>
+      <c r="E13" s="134"/>
       <c r="F13" s="74">
         <v>10</v>
       </c>
@@ -11125,8 +11973,8 @@
       <c r="Q13" s="59"/>
     </row>
     <row r="14" spans="4:22" ht="40" customHeight="1">
-      <c r="D14" s="127"/>
-      <c r="E14" s="127"/>
+      <c r="D14" s="134"/>
+      <c r="E14" s="134"/>
       <c r="F14" s="74">
         <v>10.5</v>
       </c>
@@ -11160,8 +12008,8 @@
       <c r="Q14" s="59"/>
     </row>
     <row r="15" spans="4:22" ht="40" customHeight="1">
-      <c r="D15" s="127"/>
-      <c r="E15" s="127"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="134"/>
       <c r="F15" s="74">
         <v>11</v>
       </c>
@@ -11195,8 +12043,8 @@
       <c r="Q15" s="59"/>
     </row>
     <row r="16" spans="4:22" ht="40" customHeight="1">
-      <c r="D16" s="127"/>
-      <c r="E16" s="127"/>
+      <c r="D16" s="134"/>
+      <c r="E16" s="134"/>
       <c r="F16" s="74">
         <v>11.5</v>
       </c>
@@ -11230,8 +12078,8 @@
       <c r="Q16" s="59"/>
     </row>
     <row r="17" spans="4:20" ht="40" customHeight="1">
-      <c r="D17" s="127"/>
-      <c r="E17" s="127"/>
+      <c r="D17" s="134"/>
+      <c r="E17" s="134"/>
       <c r="F17" s="79">
         <v>12</v>
       </c>
@@ -11264,8 +12112,8 @@
       <c r="Q17" s="59"/>
     </row>
     <row r="18" spans="4:20" ht="40" customHeight="1">
-      <c r="D18" s="127"/>
-      <c r="E18" s="127"/>
+      <c r="D18" s="134"/>
+      <c r="E18" s="134"/>
       <c r="F18" s="74">
         <v>12.5</v>
       </c>
@@ -11299,8 +12147,8 @@
       <c r="Q18" s="59"/>
     </row>
     <row r="19" spans="4:20" ht="40" customHeight="1">
-      <c r="D19" s="127"/>
-      <c r="E19" s="127"/>
+      <c r="D19" s="134"/>
+      <c r="E19" s="134"/>
       <c r="F19" s="74">
         <v>13</v>
       </c>
@@ -11337,8 +12185,8 @@
       <c r="T19" s="22"/>
     </row>
     <row r="20" spans="4:20" ht="40" customHeight="1">
-      <c r="D20" s="127"/>
-      <c r="E20" s="127"/>
+      <c r="D20" s="134"/>
+      <c r="E20" s="134"/>
       <c r="F20" s="74">
         <v>13.5</v>
       </c>
@@ -11375,8 +12223,8 @@
       <c r="T20" s="22"/>
     </row>
     <row r="21" spans="4:20" ht="40" customHeight="1">
-      <c r="D21" s="127"/>
-      <c r="E21" s="127"/>
+      <c r="D21" s="134"/>
+      <c r="E21" s="134"/>
       <c r="F21" s="74">
         <v>14</v>
       </c>
@@ -11412,10 +12260,10 @@
       <c r="T21" s="22"/>
     </row>
     <row r="22" spans="4:20" ht="42" customHeight="1">
-      <c r="D22" s="128" t="s">
+      <c r="D22" s="135" t="s">
         <v>98</v>
       </c>
-      <c r="E22" s="131" t="s">
+      <c r="E22" s="138" t="s">
         <v>55</v>
       </c>
       <c r="F22" s="88">
@@ -11455,8 +12303,8 @@
       <c r="T22" s="22"/>
     </row>
     <row r="23" spans="4:20" ht="40" customHeight="1">
-      <c r="D23" s="129"/>
-      <c r="E23" s="132"/>
+      <c r="D23" s="136"/>
+      <c r="E23" s="139"/>
       <c r="F23" s="88">
         <f t="shared" si="5"/>
         <v>16.648899610038097</v>
@@ -11494,8 +12342,8 @@
       <c r="T23" s="22"/>
     </row>
     <row r="24" spans="4:20" ht="40" customHeight="1">
-      <c r="D24" s="129"/>
-      <c r="E24" s="132"/>
+      <c r="D24" s="136"/>
+      <c r="E24" s="139"/>
       <c r="F24" s="88">
         <f t="shared" si="5"/>
         <v>18.155753765114138</v>
@@ -11533,8 +12381,8 @@
       <c r="T24" s="22"/>
     </row>
     <row r="25" spans="4:20" ht="40" customHeight="1">
-      <c r="D25" s="129"/>
-      <c r="E25" s="132"/>
+      <c r="D25" s="136"/>
+      <c r="E25" s="139"/>
       <c r="F25" s="88">
         <f t="shared" si="5"/>
         <v>19.798989873223334</v>
@@ -11572,8 +12420,8 @@
       <c r="T25" s="22"/>
     </row>
     <row r="26" spans="4:20" ht="40" customHeight="1">
-      <c r="D26" s="129"/>
-      <c r="E26" s="132"/>
+      <c r="D26" s="136"/>
+      <c r="E26" s="139"/>
       <c r="F26" s="88">
         <f t="shared" si="5"/>
         <v>21.590951555711175</v>
@@ -11611,8 +12459,8 @@
       <c r="T26" s="22"/>
     </row>
     <row r="27" spans="4:20" ht="40" customHeight="1">
-      <c r="D27" s="129"/>
-      <c r="E27" s="132"/>
+      <c r="D27" s="136"/>
+      <c r="E27" s="139"/>
       <c r="F27" s="88">
         <f t="shared" si="5"/>
         <v>23.545099627104012</v>
@@ -11650,8 +12498,8 @@
       <c r="T27" s="22"/>
     </row>
     <row r="28" spans="4:20" ht="40" customHeight="1">
-      <c r="D28" s="129"/>
-      <c r="E28" s="132"/>
+      <c r="D28" s="136"/>
+      <c r="E28" s="139"/>
       <c r="F28" s="88">
         <f t="shared" si="5"/>
         <v>25.676113209730801</v>
@@ -11686,8 +12534,8 @@
       <c r="Q28" s="59"/>
     </row>
     <row r="29" spans="4:20" ht="40" customHeight="1">
-      <c r="D29" s="129"/>
-      <c r="E29" s="132"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="139"/>
       <c r="F29" s="88">
         <f t="shared" si="5"/>
         <v>28.000000000000007</v>
@@ -11722,8 +12570,8 @@
       <c r="Q29" s="59"/>
     </row>
     <row r="30" spans="4:20" ht="40" customHeight="1">
-      <c r="D30" s="129"/>
-      <c r="E30" s="132"/>
+      <c r="D30" s="136"/>
+      <c r="E30" s="139"/>
       <c r="F30" s="88">
         <f t="shared" si="5"/>
         <v>30.534216514627222</v>
@@ -11758,8 +12606,8 @@
       <c r="Q30" s="59"/>
     </row>
     <row r="31" spans="4:20" ht="40" customHeight="1">
-      <c r="D31" s="129"/>
-      <c r="E31" s="132"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="139"/>
       <c r="F31" s="88">
         <f t="shared" si="5"/>
         <v>33.2977992200762</v>
@@ -11794,8 +12642,8 @@
       <c r="Q31" s="59"/>
     </row>
     <row r="32" spans="4:20" ht="40" customHeight="1">
-      <c r="D32" s="129"/>
-      <c r="E32" s="132"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="139"/>
       <c r="F32" s="88">
         <f t="shared" si="5"/>
         <v>36.311507530228283</v>
@@ -11830,8 +12678,8 @@
       <c r="Q32" s="59"/>
     </row>
     <row r="33" spans="4:17" ht="40" customHeight="1">
-      <c r="D33" s="129"/>
-      <c r="E33" s="132"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="139"/>
       <c r="F33" s="88">
         <f t="shared" si="5"/>
         <v>39.597979746446676</v>
@@ -11866,8 +12714,8 @@
       <c r="Q33" s="59"/>
     </row>
     <row r="34" spans="4:17" ht="40" customHeight="1">
-      <c r="D34" s="129"/>
-      <c r="E34" s="132"/>
+      <c r="D34" s="136"/>
+      <c r="E34" s="139"/>
       <c r="F34" s="88">
         <f t="shared" si="5"/>
         <v>43.181903111422358</v>
@@ -11902,8 +12750,8 @@
       <c r="Q34" s="59"/>
     </row>
     <row r="35" spans="4:17" ht="40" customHeight="1">
-      <c r="D35" s="129"/>
-      <c r="E35" s="132"/>
+      <c r="D35" s="136"/>
+      <c r="E35" s="139"/>
       <c r="F35" s="88">
         <f t="shared" si="5"/>
         <v>47.090199254208031</v>
@@ -11938,8 +12786,8 @@
       <c r="Q35" s="59"/>
     </row>
     <row r="36" spans="4:17" ht="40" customHeight="1">
-      <c r="D36" s="129"/>
-      <c r="E36" s="132"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="139"/>
       <c r="F36" s="88">
         <f t="shared" si="5"/>
         <v>51.352226419461608</v>
@@ -11974,8 +12822,8 @@
       <c r="Q36" s="59"/>
     </row>
     <row r="37" spans="4:17" ht="40" customHeight="1">
-      <c r="D37" s="130"/>
-      <c r="E37" s="133"/>
+      <c r="D37" s="137"/>
+      <c r="E37" s="140"/>
       <c r="F37" s="88">
         <f t="shared" si="5"/>
         <v>56.000000000000021</v>
@@ -12010,8 +12858,8 @@
       <c r="Q37" s="59"/>
     </row>
     <row r="38" spans="4:17" ht="40" customHeight="1">
-      <c r="D38" s="130"/>
-      <c r="E38" s="133"/>
+      <c r="D38" s="137"/>
+      <c r="E38" s="140"/>
       <c r="F38" s="88">
         <f t="shared" si="5"/>
         <v>61.068433029254457</v>
@@ -12046,8 +12894,8 @@
       <c r="Q38" s="59"/>
     </row>
     <row r="39" spans="4:17" ht="40" customHeight="1">
-      <c r="D39" s="130"/>
-      <c r="E39" s="133"/>
+      <c r="D39" s="137"/>
+      <c r="E39" s="140"/>
       <c r="F39" s="88">
         <f t="shared" si="5"/>
         <v>66.595598440152415</v>
@@ -12082,8 +12930,8 @@
       <c r="Q39" s="59"/>
     </row>
     <row r="40" spans="4:17" ht="40" customHeight="1">
-      <c r="D40" s="130"/>
-      <c r="E40" s="133"/>
+      <c r="D40" s="137"/>
+      <c r="E40" s="140"/>
       <c r="F40" s="88">
         <f t="shared" si="5"/>
         <v>72.623015060456581</v>
@@ -12118,8 +12966,8 @@
       <c r="Q40" s="59"/>
     </row>
     <row r="41" spans="4:17" ht="40" customHeight="1">
-      <c r="D41" s="130"/>
-      <c r="E41" s="133"/>
+      <c r="D41" s="137"/>
+      <c r="E41" s="140"/>
       <c r="F41" s="88">
         <f t="shared" si="5"/>
         <v>79.195959492893365</v>
@@ -12154,8 +13002,8 @@
       <c r="Q41" s="59"/>
     </row>
     <row r="42" spans="4:17" ht="40" customHeight="1">
-      <c r="D42" s="130"/>
-      <c r="E42" s="133"/>
+      <c r="D42" s="137"/>
+      <c r="E42" s="140"/>
       <c r="F42" s="88">
         <f t="shared" si="5"/>
         <v>86.36380622284473</v>
@@ -12190,8 +13038,8 @@
       <c r="Q42" s="59"/>
     </row>
     <row r="43" spans="4:17" ht="40" customHeight="1">
-      <c r="D43" s="130"/>
-      <c r="E43" s="133"/>
+      <c r="D43" s="137"/>
+      <c r="E43" s="140"/>
       <c r="F43" s="88">
         <f t="shared" si="5"/>
         <v>94.180398508416076</v>
@@ -12226,8 +13074,8 @@
       <c r="Q43" s="59"/>
     </row>
     <row r="44" spans="4:17" ht="40" customHeight="1">
-      <c r="D44" s="130"/>
-      <c r="E44" s="133"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="140"/>
       <c r="F44" s="88">
         <f t="shared" si="5"/>
         <v>102.70445283892323</v>
@@ -12262,8 +13110,8 @@
       <c r="Q44" s="59"/>
     </row>
     <row r="45" spans="4:17" ht="40" customHeight="1">
-      <c r="D45" s="130"/>
-      <c r="E45" s="133"/>
+      <c r="D45" s="137"/>
+      <c r="E45" s="140"/>
       <c r="F45" s="88">
         <f t="shared" si="5"/>
         <v>112.00000000000006</v>
@@ -12298,8 +13146,8 @@
       <c r="Q45" s="59"/>
     </row>
     <row r="46" spans="4:17" ht="40" customHeight="1">
-      <c r="D46" s="130"/>
-      <c r="E46" s="133"/>
+      <c r="D46" s="137"/>
+      <c r="E46" s="140"/>
       <c r="F46" s="88">
         <f t="shared" ref="F46:H53" si="7">F45*$T$11</f>
         <v>122.13686605850893</v>
@@ -12334,8 +13182,8 @@
       <c r="Q46" s="59"/>
     </row>
     <row r="47" spans="4:17" ht="40" customHeight="1">
-      <c r="D47" s="130"/>
-      <c r="E47" s="133"/>
+      <c r="D47" s="137"/>
+      <c r="E47" s="140"/>
       <c r="F47" s="88">
         <f t="shared" si="7"/>
         <v>133.19119688030483</v>
@@ -12370,8 +13218,8 @@
       <c r="Q47" s="59"/>
     </row>
     <row r="48" spans="4:17" ht="40" customHeight="1">
-      <c r="D48" s="130"/>
-      <c r="E48" s="133"/>
+      <c r="D48" s="137"/>
+      <c r="E48" s="140"/>
       <c r="F48" s="88">
         <f t="shared" si="7"/>
         <v>145.24603012091316</v>
@@ -12406,8 +13254,8 @@
       <c r="Q48" s="59"/>
     </row>
     <row r="49" spans="4:17" ht="40" customHeight="1">
-      <c r="D49" s="130"/>
-      <c r="E49" s="133"/>
+      <c r="D49" s="137"/>
+      <c r="E49" s="140"/>
       <c r="F49" s="88">
         <f t="shared" si="7"/>
         <v>158.39191898578673</v>
@@ -12442,8 +13290,8 @@
       <c r="Q49" s="59"/>
     </row>
     <row r="50" spans="4:17" ht="40" customHeight="1">
-      <c r="D50" s="130"/>
-      <c r="E50" s="133"/>
+      <c r="D50" s="137"/>
+      <c r="E50" s="140"/>
       <c r="F50" s="88">
         <f t="shared" si="7"/>
         <v>172.72761244568946</v>
@@ -12478,8 +13326,8 @@
       <c r="Q50" s="59"/>
     </row>
     <row r="51" spans="4:17" ht="40" customHeight="1">
-      <c r="D51" s="130"/>
-      <c r="E51" s="133"/>
+      <c r="D51" s="137"/>
+      <c r="E51" s="140"/>
       <c r="F51" s="88">
         <f t="shared" si="7"/>
         <v>188.36079701683215</v>
@@ -12514,8 +13362,8 @@
       <c r="Q51" s="59"/>
     </row>
     <row r="52" spans="4:17" ht="40" customHeight="1">
-      <c r="D52" s="130"/>
-      <c r="E52" s="133"/>
+      <c r="D52" s="137"/>
+      <c r="E52" s="140"/>
       <c r="F52" s="88">
         <f t="shared" si="7"/>
         <v>205.40890567784646</v>
@@ -12550,8 +13398,8 @@
       <c r="Q52" s="59"/>
     </row>
     <row r="53" spans="4:17" ht="40" customHeight="1" thickBot="1">
-      <c r="D53" s="130"/>
-      <c r="E53" s="133"/>
+      <c r="D53" s="137"/>
+      <c r="E53" s="140"/>
       <c r="F53" s="89">
         <f t="shared" si="7"/>
         <v>224.00000000000011</v>

</xml_diff>